<commit_message>
Se termina de agregar archivos recibidos por victor
</commit_message>
<xml_diff>
--- a/Modulo 2/OrganizacionEjercicios.xlsx
+++ b/Modulo 2/OrganizacionEjercicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyes\Documents\GitHub\CursoIoTCorfo\Modulo 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6566CA-B45E-4B20-A99C-796C25D23F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028C11F0-C15F-4C6D-8C30-BFC140D1933B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{0E82C134-1E43-4CAB-B30A-C563DAA28B82}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="22">
   <si>
     <t>Clase 2</t>
   </si>
@@ -94,6 +94,12 @@
   <si>
     <t>Alex</t>
   </si>
+  <si>
+    <t>Alvaro</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
 </sst>
 </file>
 
@@ -277,7 +283,504 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="70">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -589,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C8765D-BADE-4F4C-9909-5A90AB41C66D}">
   <dimension ref="A2:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +1250,9 @@
       <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
@@ -757,7 +1262,9 @@
       <c r="L4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="N4" s="1" t="s">
         <v>5</v>
       </c>
@@ -767,7 +1274,9 @@
       <c r="P4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="1"/>
+      <c r="Q4" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="R4" s="1" t="s">
         <v>5</v>
       </c>
@@ -777,7 +1286,9 @@
       <c r="T4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U4" s="1"/>
+      <c r="U4" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="V4" s="1" t="s">
         <v>5</v>
       </c>
@@ -785,7 +1296,9 @@
       <c r="X4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="1"/>
+      <c r="Y4" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -810,7 +1323,9 @@
       <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
@@ -820,7 +1335,9 @@
       <c r="L5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="N5" s="1" t="s">
         <v>6</v>
       </c>
@@ -830,7 +1347,9 @@
       <c r="P5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="R5" s="1" t="s">
         <v>6</v>
       </c>
@@ -873,7 +1392,9 @@
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J6" s="1" t="s">
         <v>7</v>
       </c>
@@ -883,7 +1404,9 @@
       <c r="L6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="N6" s="1" t="s">
         <v>7</v>
       </c>
@@ -893,7 +1416,9 @@
       <c r="P6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="1"/>
+      <c r="Q6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -924,7 +1449,9 @@
       <c r="H7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>8</v>
       </c>
@@ -934,7 +1461,9 @@
       <c r="L7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -969,7 +1498,9 @@
       <c r="H8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1074,7 +1605,9 @@
       <c r="H11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1092,7 +1625,9 @@
       <c r="P11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q11" s="1"/>
+      <c r="Q11" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="R11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1133,7 +1668,9 @@
       <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1151,7 +1688,9 @@
       <c r="P12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q12" s="1"/>
+      <c r="Q12" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="R12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1159,7 +1698,9 @@
       <c r="T12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U12" s="1"/>
+      <c r="U12" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="V12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1167,7 +1708,9 @@
       <c r="X12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Y12" s="1"/>
+      <c r="Y12" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -1192,7 +1735,9 @@
       <c r="H13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1237,7 +1782,9 @@
       <c r="H14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1336,7 +1883,9 @@
       <c r="H17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1371,7 +1920,9 @@
       <c r="H18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1457,17 +2008,157 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="V2:Y2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="S11:S12">
+    <cfRule type="expression" dxfId="27" priority="33">
+      <formula>ISBLANK(S11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U11:U12">
+    <cfRule type="expression" dxfId="26" priority="27">
+      <formula>ISBLANK(U11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U4:U5">
+    <cfRule type="expression" dxfId="25" priority="26">
+      <formula>ISBLANK(U4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W4:W5">
+    <cfRule type="expression" dxfId="24" priority="25">
+      <formula>ISBLANK(W4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y4:Y5">
+    <cfRule type="expression" dxfId="23" priority="24">
+      <formula>ISBLANK(Y4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W11:W12">
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>ISBLANK(W11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y11:Y12">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>ISBLANK(Y11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C9">
+    <cfRule type="expression" dxfId="20" priority="21">
+      <formula>ISBLANK(C4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C15">
+    <cfRule type="expression" dxfId="19" priority="20">
+      <formula>ISBLANK(C11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E9">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>ISBLANK(E4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E15">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>ISBLANK(E11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G8">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>ISBLANK(G4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G14">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>ISBLANK(G11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17:G18">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>ISBLANK(G17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I8">
+    <cfRule type="expression" dxfId="13" priority="14">
+      <formula>ISBLANK(I4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I14">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>ISBLANK(I11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17:I18">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>ISBLANK(I17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17:K20">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>ISBLANK(K17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:M20">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>ISBLANK(M17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K7">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>ISBLANK(K4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11:K14">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>ISBLANK(K11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:M14">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>ISBLANK(M11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M7">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>ISBLANK(M4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:O6">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>ISBLANK(O4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O11:O12">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>ISBLANK(O11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q11:Q12">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>ISBLANK(Q11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4:Q6">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>ISBLANK(Q4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S4:S5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>ISBLANK(S4)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>